<commit_message>
Added Food Waste Tab
</commit_message>
<xml_diff>
--- a/pythonshinyproject/dashboard/data/brightway/Scenarios Database.xlsx
+++ b/pythonshinyproject/dashboard/data/brightway/Scenarios Database.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="K70" sqref="K70"/>
@@ -1818,6 +1818,287 @@
     </row>
     <row r="68">
       <c r="D68" s="9" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>production amount</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Exchanges</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>reference product</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>OFMSW</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Scenarios</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>production</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Closed-tunnel Composter</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>OFMSW</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>OWM Facilities</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>technosphere</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>OFMSW</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>OWM Facilities</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>technosphere</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated portion of readme
</commit_message>
<xml_diff>
--- a/pythonshinyproject/dashboard/data/brightway/Scenarios Database.xlsx
+++ b/pythonshinyproject/dashboard/data/brightway/Scenarios Database.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="K70" sqref="K70"/>
@@ -1830,13 +1830,6 @@
           <t>Test</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1849,13 +1842,6 @@
           <t>Test</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1868,13 +1854,6 @@
           <t>CA-QC</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1887,13 +1866,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1906,39 +1878,14 @@
           <t>tonne</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr"/>
-      <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
-    </row>
+    </row>
+    <row r="74"/>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
           <t>Exchanges</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2023,8 +1970,6 @@
           <t>production</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2060,8 +2005,6 @@
           <t>technosphere</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2097,8 +2040,250 @@
           <t>technosphere</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>production amount</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Exchanges</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>reference product</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>OFMSW</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Scenarios</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>production</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Landfill_saint sophie</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>OFMSW</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>CA-QC</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>OWM Facilities</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>technosphere</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>